<commit_message>
integrate database all in one
</commit_message>
<xml_diff>
--- a/database/industries/ghaza/gheshasfa/income/quarterly/dollar.xlsx
+++ b/database/industries/ghaza/gheshasfa/income/quarterly/dollar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VAHID\Desktop\Trade\database\industries\ghaza\gheshasfa\income\quarterly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Users\EBRAHIMI\Desktop\Trade\database\industries\ghaza\gheshasfa\income\quarterly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E92F07B-5567-4665-BC6E-1D70FC16DD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C564E4D5-AA65-4422-AD6F-0A99F100CBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>

</xml_diff>